<commit_message>
edited one data point by comparing wtih original datasheets
</commit_message>
<xml_diff>
--- a/biol_402_epiphyte_shoots.xlsx
+++ b/biol_402_epiphyte_shoots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryoconnor/Github/Biol 402/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryoconnor/Github/Biol402/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDAB48F-AA81-2846-9115-8757B7380854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26CD0E9-1FAF-8340-AA2D-2D51055FDDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="22460" windowHeight="16500" xr2:uid="{EBDD8445-C656-B04F-BA9A-67D36C56F22E}"/>
+    <workbookView xWindow="1140" yWindow="500" windowWidth="34980" windowHeight="17040" xr2:uid="{EBDD8445-C656-B04F-BA9A-67D36C56F22E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21:XFD21"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>